<commit_message>
Antibody calculations for tomorrow.
</commit_message>
<xml_diff>
--- a/2025_SFC_Panels.xlsx
+++ b/2025_SFC_Panels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drach\Documents\AlphaBeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4D5307-B8D9-40D4-872D-FB90E6FD35E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A9BBA-5C4E-453B-A519-873665C605CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallPanel" sheetId="50" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="421">
   <si>
     <t>Esosa Practice Experiment #1</t>
   </si>
@@ -1646,7 +1646,16 @@
     <t>&lt;0.8&gt;</t>
   </si>
   <si>
-    <t>July 26th, 2025</t>
+    <t>July 29th, 2025</t>
+  </si>
+  <si>
+    <t>Wash with 1 ml PBS, spin down 1300rpm 8min</t>
+  </si>
+  <si>
+    <t>750 ul of LiveDead mix (1:2500) @RT for 15min</t>
+  </si>
+  <si>
+    <t>0.75 ml Nuclear FixPerm, incubate @ 4C for  30min</t>
   </si>
 </sst>
 </file>
@@ -3030,7 +3039,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="650">
+  <cellXfs count="649">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4775,9 +4784,6 @@
     <xf numFmtId="0" fontId="77" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="52" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="79" fillId="16" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4842,22 +4848,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5255,10 +5261,10 @@
       <c r="H1" s="400" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="618" t="s">
+      <c r="Q1" s="617" t="s">
         <v>317</v>
       </c>
-      <c r="R1" s="618"/>
+      <c r="R1" s="617"/>
       <c r="S1" s="400"/>
     </row>
     <row r="2" spans="2:25" ht="90.75" customHeight="1">
@@ -7317,10 +7323,10 @@
       </c>
       <c r="D57" s="482"/>
       <c r="E57" s="483"/>
-      <c r="F57" s="619" t="s">
+      <c r="F57" s="618" t="s">
         <v>194</v>
       </c>
-      <c r="G57" s="619"/>
+      <c r="G57" s="618"/>
       <c r="H57" s="484">
         <f>SUM(H4:H56)</f>
         <v>0</v>
@@ -7366,10 +7372,10 @@
       <c r="C58" s="492"/>
       <c r="D58" s="549"/>
       <c r="E58" s="550"/>
-      <c r="F58" s="620" t="s">
+      <c r="F58" s="619" t="s">
         <v>196</v>
       </c>
-      <c r="G58" s="620"/>
+      <c r="G58" s="619"/>
       <c r="H58" s="493">
         <f>SUM(20.5-H57)</f>
         <v>20.5</v>
@@ -7416,19 +7422,19 @@
       <c r="C59" s="497"/>
       <c r="D59" s="498"/>
       <c r="E59" s="499"/>
-      <c r="F59" s="621" t="s">
+      <c r="F59" s="620" t="s">
         <v>198</v>
       </c>
-      <c r="G59" s="621"/>
+      <c r="G59" s="620"/>
       <c r="H59" s="500">
         <f>(H57+H58)-1</f>
         <v>19.5</v>
       </c>
       <c r="I59" s="474"/>
-      <c r="J59" s="622" t="s">
+      <c r="J59" s="621" t="s">
         <v>198</v>
       </c>
-      <c r="K59" s="622"/>
+      <c r="K59" s="621"/>
       <c r="L59" s="527">
         <f>(L57+L58)-3</f>
         <v>23.700000000000003</v>
@@ -8297,16 +8303,16 @@
       <c r="L2" s="202"/>
     </row>
     <row r="3" spans="2:12" ht="21">
-      <c r="B3" s="623" t="s">
+      <c r="B3" s="622" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="624"/>
-      <c r="D3" s="624"/>
-      <c r="E3" s="624"/>
-      <c r="F3" s="624"/>
-      <c r="G3" s="624"/>
-      <c r="H3" s="624"/>
-      <c r="I3" s="625"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
+      <c r="G3" s="623"/>
+      <c r="H3" s="623"/>
+      <c r="I3" s="624"/>
       <c r="J3" s="202"/>
       <c r="K3" s="202"/>
       <c r="L3" s="202"/>
@@ -8711,14 +8717,14 @@
       <c r="L19" s="202"/>
     </row>
     <row r="20" spans="2:12" ht="21">
-      <c r="B20" s="626" t="s">
+      <c r="B20" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="627"/>
-      <c r="D20" s="627"/>
-      <c r="E20" s="627"/>
-      <c r="F20" s="627"/>
-      <c r="G20" s="627"/>
+      <c r="C20" s="626"/>
+      <c r="D20" s="626"/>
+      <c r="E20" s="626"/>
+      <c r="F20" s="626"/>
+      <c r="G20" s="626"/>
       <c r="H20" s="189">
         <f>SUM(H5:H19)</f>
         <v>19.2</v>
@@ -8732,14 +8738,14 @@
       <c r="L20" s="202"/>
     </row>
     <row r="21" spans="2:12" ht="21">
-      <c r="B21" s="626" t="s">
+      <c r="B21" s="625" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="627"/>
-      <c r="D21" s="627"/>
-      <c r="E21" s="627"/>
-      <c r="F21" s="627"/>
-      <c r="G21" s="627"/>
+      <c r="C21" s="626"/>
+      <c r="D21" s="626"/>
+      <c r="E21" s="626"/>
+      <c r="F21" s="626"/>
+      <c r="G21" s="626"/>
       <c r="H21" s="189">
         <f>50.5-H20</f>
         <v>31.3</v>
@@ -8753,14 +8759,14 @@
       <c r="L21" s="202"/>
     </row>
     <row r="22" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B22" s="628" t="s">
+      <c r="B22" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="629"/>
-      <c r="D22" s="629"/>
-      <c r="E22" s="629"/>
-      <c r="F22" s="629"/>
-      <c r="G22" s="629"/>
+      <c r="C22" s="628"/>
+      <c r="D22" s="628"/>
+      <c r="E22" s="628"/>
+      <c r="F22" s="628"/>
+      <c r="G22" s="628"/>
       <c r="H22" s="348">
         <f>(H20+H21)-1</f>
         <v>49.5</v>
@@ -10417,10 +10423,10 @@
         <f>K35*L2</f>
         <v>36</v>
       </c>
-      <c r="M35" s="634" t="s">
+      <c r="M35" s="633" t="s">
         <v>194</v>
       </c>
-      <c r="N35" s="635"/>
+      <c r="N35" s="634"/>
       <c r="O35" s="208">
         <f>SUM(O3:O34)</f>
         <v>17.8</v>
@@ -10471,10 +10477,10 @@
         <f>K36*L2</f>
         <v>87</v>
       </c>
-      <c r="M36" s="632" t="s">
+      <c r="M36" s="631" t="s">
         <v>197</v>
       </c>
-      <c r="N36" s="633"/>
+      <c r="N36" s="632"/>
       <c r="O36" s="215">
         <v>50</v>
       </c>
@@ -10504,19 +10510,19 @@
       <c r="C37" s="57"/>
       <c r="G37" s="37"/>
       <c r="H37" s="48"/>
-      <c r="I37" s="630" t="s">
+      <c r="I37" s="629" t="s">
         <v>198</v>
       </c>
-      <c r="J37" s="631"/>
+      <c r="J37" s="630"/>
       <c r="K37" s="227">
         <f>(K35+K36)-1</f>
         <v>19.5</v>
       </c>
       <c r="L37" s="220"/>
-      <c r="M37" s="636" t="s">
+      <c r="M37" s="635" t="s">
         <v>198</v>
       </c>
-      <c r="N37" s="637"/>
+      <c r="N37" s="636"/>
       <c r="O37" s="219">
         <f>(O35+O36)-3</f>
         <v>64.8</v>
@@ -10966,19 +10972,19 @@
       <c r="R34" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="638" t="s">
+      <c r="T34" s="642" t="s">
         <v>205</v>
       </c>
-      <c r="U34" s="638"/>
-      <c r="V34" s="638"/>
-      <c r="W34" s="638"/>
+      <c r="U34" s="642"/>
+      <c r="V34" s="642"/>
+      <c r="W34" s="642"/>
       <c r="X34" s="87"/>
-      <c r="Y34" s="638" t="s">
+      <c r="Y34" s="642" t="s">
         <v>206</v>
       </c>
-      <c r="Z34" s="638"/>
-      <c r="AA34" s="638"/>
-      <c r="AB34" s="638"/>
+      <c r="Z34" s="642"/>
+      <c r="AA34" s="642"/>
+      <c r="AB34" s="642"/>
       <c r="AH34" s="87"/>
     </row>
     <row r="35" spans="2:34">
@@ -11092,7 +11098,7 @@
       <c r="R36" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="T36" s="639" t="s">
+      <c r="T36" s="638" t="s">
         <v>210</v>
       </c>
       <c r="U36" s="363" t="s">
@@ -11105,7 +11111,7 @@
         <v>38</v>
       </c>
       <c r="X36" s="87"/>
-      <c r="Y36" s="639" t="s">
+      <c r="Y36" s="638" t="s">
         <v>210</v>
       </c>
       <c r="Z36" s="363" t="s">
@@ -11159,7 +11165,7 @@
         <v>9</v>
       </c>
       <c r="R37" s="145"/>
-      <c r="T37" s="641"/>
+      <c r="T37" s="639"/>
       <c r="U37" s="363" t="s">
         <v>212</v>
       </c>
@@ -11170,7 +11176,7 @@
         <v>44</v>
       </c>
       <c r="X37" s="87"/>
-      <c r="Y37" s="641"/>
+      <c r="Y37" s="639"/>
       <c r="Z37" s="363" t="s">
         <v>212</v>
       </c>
@@ -11293,7 +11299,7 @@
         <v>87</v>
       </c>
       <c r="R39" s="147"/>
-      <c r="T39" s="639" t="s">
+      <c r="T39" s="638" t="s">
         <v>216</v>
       </c>
       <c r="U39" s="81" t="s">
@@ -11306,7 +11312,7 @@
         <v>219</v>
       </c>
       <c r="X39" s="87"/>
-      <c r="Y39" s="639" t="s">
+      <c r="Y39" s="638" t="s">
         <v>216</v>
       </c>
       <c r="Z39" s="81" t="s">
@@ -11427,7 +11433,7 @@
       <c r="R41" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="T41" s="639" t="s">
+      <c r="T41" s="638" t="s">
         <v>225</v>
       </c>
       <c r="U41" s="364" t="s">
@@ -11440,7 +11446,7 @@
         <v>227</v>
       </c>
       <c r="X41" s="87"/>
-      <c r="Y41" s="639" t="s">
+      <c r="Y41" s="638" t="s">
         <v>225</v>
       </c>
       <c r="Z41" s="364" t="s">
@@ -11496,7 +11502,7 @@
       <c r="R42" s="108" t="s">
         <v>108</v>
       </c>
-      <c r="T42" s="641"/>
+      <c r="T42" s="639"/>
       <c r="U42" s="365" t="s">
         <v>228</v>
       </c>
@@ -11505,7 +11511,7 @@
       </c>
       <c r="W42" s="370"/>
       <c r="X42" s="87"/>
-      <c r="Y42" s="641"/>
+      <c r="Y42" s="639"/>
       <c r="Z42" s="365" t="s">
         <v>228</v>
       </c>
@@ -11622,7 +11628,7 @@
       <c r="R44" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="T44" s="639" t="s">
+      <c r="T44" s="638" t="s">
         <v>236</v>
       </c>
       <c r="U44" s="82" t="s">
@@ -11634,7 +11640,7 @@
       <c r="W44" s="369" t="s">
         <v>238</v>
       </c>
-      <c r="Y44" s="639" t="s">
+      <c r="Y44" s="638" t="s">
         <v>236</v>
       </c>
       <c r="Z44" s="82" t="s">
@@ -11687,7 +11693,7 @@
         <v>114</v>
       </c>
       <c r="R45" s="135"/>
-      <c r="T45" s="642"/>
+      <c r="T45" s="641"/>
       <c r="U45" s="89" t="s">
         <v>241</v>
       </c>
@@ -11698,7 +11704,7 @@
         <v>41</v>
       </c>
       <c r="X45" s="87"/>
-      <c r="Y45" s="642"/>
+      <c r="Y45" s="641"/>
       <c r="Z45" s="89" t="s">
         <v>241</v>
       </c>
@@ -11801,19 +11807,19 @@
       <c r="R47" s="135" t="s">
         <v>245</v>
       </c>
-      <c r="T47" s="638" t="s">
+      <c r="T47" s="642" t="s">
         <v>246</v>
       </c>
-      <c r="U47" s="638"/>
-      <c r="V47" s="638"/>
-      <c r="W47" s="638"/>
+      <c r="U47" s="642"/>
+      <c r="V47" s="642"/>
+      <c r="W47" s="642"/>
       <c r="X47" s="87"/>
-      <c r="Y47" s="638" t="s">
+      <c r="Y47" s="642" t="s">
         <v>247</v>
       </c>
-      <c r="Z47" s="638"/>
-      <c r="AA47" s="638"/>
-      <c r="AB47" s="638"/>
+      <c r="Z47" s="642"/>
+      <c r="AA47" s="642"/>
+      <c r="AB47" s="642"/>
     </row>
     <row r="48" spans="2:34">
       <c r="B48" s="150"/>
@@ -11925,7 +11931,7 @@
       <c r="R49" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="T49" s="639" t="s">
+      <c r="T49" s="638" t="s">
         <v>210</v>
       </c>
       <c r="U49" s="83" t="s">
@@ -11938,7 +11944,7 @@
         <v>238</v>
       </c>
       <c r="X49" s="87"/>
-      <c r="Y49" s="639" t="s">
+      <c r="Y49" s="638" t="s">
         <v>210</v>
       </c>
       <c r="Z49" s="83" t="s">
@@ -11993,7 +11999,7 @@
       <c r="R50" s="103" t="s">
         <v>252</v>
       </c>
-      <c r="T50" s="641"/>
+      <c r="T50" s="639"/>
       <c r="U50" s="83" t="s">
         <v>212</v>
       </c>
@@ -12004,7 +12010,7 @@
         <v>29</v>
       </c>
       <c r="X50" s="87"/>
-      <c r="Y50" s="641"/>
+      <c r="Y50" s="639"/>
       <c r="Z50" s="83" t="s">
         <v>212</v>
       </c>
@@ -12119,7 +12125,7 @@
       <c r="R52" s="114" t="s">
         <v>255</v>
       </c>
-      <c r="T52" s="639" t="s">
+      <c r="T52" s="638" t="s">
         <v>216</v>
       </c>
       <c r="U52" s="81" t="s">
@@ -12132,7 +12138,7 @@
         <v>219</v>
       </c>
       <c r="X52" s="87"/>
-      <c r="Y52" s="639" t="s">
+      <c r="Y52" s="638" t="s">
         <v>216</v>
       </c>
       <c r="Z52" s="81" t="s">
@@ -12251,7 +12257,7 @@
       <c r="R54" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="T54" s="639" t="s">
+      <c r="T54" s="638" t="s">
         <v>225</v>
       </c>
       <c r="U54" s="364" t="s">
@@ -12264,7 +12270,7 @@
         <v>38</v>
       </c>
       <c r="X54" s="87"/>
-      <c r="Y54" s="639" t="s">
+      <c r="Y54" s="638" t="s">
         <v>225</v>
       </c>
       <c r="Z54" s="364" t="s">
@@ -12319,7 +12325,7 @@
       <c r="R55" s="135" t="s">
         <v>264</v>
       </c>
-      <c r="T55" s="641"/>
+      <c r="T55" s="639"/>
       <c r="U55" s="365" t="s">
         <v>228</v>
       </c>
@@ -12328,7 +12334,7 @@
       </c>
       <c r="W55" s="370"/>
       <c r="X55" s="87"/>
-      <c r="Y55" s="641"/>
+      <c r="Y55" s="639"/>
       <c r="Z55" s="365" t="s">
         <v>228</v>
       </c>
@@ -12446,7 +12452,7 @@
       <c r="R57" s="135" t="s">
         <v>267</v>
       </c>
-      <c r="T57" s="639" t="s">
+      <c r="T57" s="638" t="s">
         <v>236</v>
       </c>
       <c r="U57" s="82" t="s">
@@ -12458,7 +12464,7 @@
       <c r="W57" s="369" t="s">
         <v>268</v>
       </c>
-      <c r="Y57" s="639" t="s">
+      <c r="Y57" s="638" t="s">
         <v>236</v>
       </c>
       <c r="Z57" s="82" t="s">
@@ -12513,7 +12519,7 @@
       <c r="R58" s="103" t="s">
         <v>271</v>
       </c>
-      <c r="T58" s="642"/>
+      <c r="T58" s="641"/>
       <c r="U58" s="89" t="s">
         <v>241</v>
       </c>
@@ -12523,7 +12529,7 @@
       <c r="W58" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="Y58" s="642"/>
+      <c r="Y58" s="641"/>
       <c r="Z58" s="89" t="s">
         <v>241</v>
       </c>
@@ -12617,18 +12623,18 @@
         <v>40</v>
       </c>
       <c r="R60" s="127"/>
-      <c r="T60" s="638" t="s">
+      <c r="T60" s="642" t="s">
         <v>274</v>
       </c>
-      <c r="U60" s="638"/>
-      <c r="V60" s="638"/>
-      <c r="W60" s="638"/>
-      <c r="Y60" s="638" t="s">
+      <c r="U60" s="642"/>
+      <c r="V60" s="642"/>
+      <c r="W60" s="642"/>
+      <c r="Y60" s="642" t="s">
         <v>275</v>
       </c>
-      <c r="Z60" s="638"/>
-      <c r="AA60" s="638"/>
-      <c r="AB60" s="638"/>
+      <c r="Z60" s="642"/>
+      <c r="AA60" s="642"/>
+      <c r="AB60" s="642"/>
     </row>
     <row r="61" spans="2:28" ht="19.5" customHeight="1">
       <c r="B61" s="150"/>
@@ -12745,7 +12751,7 @@
       <c r="R62" s="103" t="s">
         <v>280</v>
       </c>
-      <c r="T62" s="639" t="s">
+      <c r="T62" s="638" t="s">
         <v>210</v>
       </c>
       <c r="U62" s="83" t="s">
@@ -12757,7 +12763,7 @@
       <c r="W62" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="Y62" s="639" t="s">
+      <c r="Y62" s="638" t="s">
         <v>210</v>
       </c>
       <c r="Z62" s="83" t="s">
@@ -12812,7 +12818,7 @@
       <c r="R63" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="T63" s="641"/>
+      <c r="T63" s="639"/>
       <c r="U63" s="83" t="s">
         <v>212</v>
       </c>
@@ -12822,7 +12828,7 @@
       <c r="W63" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="Y63" s="641"/>
+      <c r="Y63" s="639"/>
       <c r="Z63" s="83" t="s">
         <v>212</v>
       </c>
@@ -12938,7 +12944,7 @@
       <c r="R65" s="148" t="s">
         <v>192</v>
       </c>
-      <c r="T65" s="639" t="s">
+      <c r="T65" s="638" t="s">
         <v>216</v>
       </c>
       <c r="U65" s="81" t="s">
@@ -12950,7 +12956,7 @@
       <c r="W65" s="369" t="s">
         <v>238</v>
       </c>
-      <c r="Y65" s="639" t="s">
+      <c r="Y65" s="638" t="s">
         <v>216</v>
       </c>
       <c r="Z65" s="81" t="s">
@@ -12986,7 +12992,7 @@
       </c>
     </row>
     <row r="67" spans="2:28">
-      <c r="T67" s="639" t="s">
+      <c r="T67" s="638" t="s">
         <v>225</v>
       </c>
       <c r="U67" s="364" t="s">
@@ -12998,7 +13004,7 @@
       <c r="W67" s="100" t="s">
         <v>281</v>
       </c>
-      <c r="Y67" s="639" t="s">
+      <c r="Y67" s="638" t="s">
         <v>225</v>
       </c>
       <c r="Z67" s="364" t="s">
@@ -13012,7 +13018,7 @@
       </c>
     </row>
     <row r="68" spans="2:28">
-      <c r="T68" s="641"/>
+      <c r="T68" s="639"/>
       <c r="U68" s="366" t="s">
         <v>228</v>
       </c>
@@ -13022,7 +13028,7 @@
       <c r="W68" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="Y68" s="641"/>
+      <c r="Y68" s="639"/>
       <c r="Z68" s="366" t="s">
         <v>228</v>
       </c>
@@ -13056,7 +13062,7 @@
       </c>
     </row>
     <row r="70" spans="2:28">
-      <c r="T70" s="639" t="s">
+      <c r="T70" s="638" t="s">
         <v>236</v>
       </c>
       <c r="U70" s="82" t="s">
@@ -13068,7 +13074,7 @@
       <c r="W70" s="369" t="s">
         <v>268</v>
       </c>
-      <c r="Y70" s="639" t="s">
+      <c r="Y70" s="638" t="s">
         <v>236</v>
       </c>
       <c r="Z70" s="82" t="s">
@@ -13082,7 +13088,7 @@
       </c>
     </row>
     <row r="71" spans="2:28" ht="16.5" thickBot="1">
-      <c r="T71" s="642"/>
+      <c r="T71" s="641"/>
       <c r="U71" s="89" t="s">
         <v>241</v>
       </c>
@@ -13092,7 +13098,7 @@
       <c r="W71" s="114" t="s">
         <v>20</v>
       </c>
-      <c r="Y71" s="642"/>
+      <c r="Y71" s="641"/>
       <c r="Z71" s="89" t="s">
         <v>241</v>
       </c>
@@ -13104,18 +13110,18 @@
       </c>
     </row>
     <row r="73" spans="2:28" ht="16.5" thickBot="1">
-      <c r="T73" s="643" t="s">
+      <c r="T73" s="637" t="s">
         <v>282</v>
       </c>
-      <c r="U73" s="643"/>
-      <c r="V73" s="643"/>
-      <c r="W73" s="643"/>
-      <c r="Y73" s="643" t="s">
+      <c r="U73" s="637"/>
+      <c r="V73" s="637"/>
+      <c r="W73" s="637"/>
+      <c r="Y73" s="637" t="s">
         <v>283</v>
       </c>
-      <c r="Z73" s="643"/>
-      <c r="AA73" s="643"/>
-      <c r="AB73" s="643"/>
+      <c r="Z73" s="637"/>
+      <c r="AA73" s="637"/>
+      <c r="AB73" s="637"/>
     </row>
     <row r="74" spans="2:28">
       <c r="T74" s="367" t="s">
@@ -13144,7 +13150,7 @@
       </c>
     </row>
     <row r="75" spans="2:28">
-      <c r="T75" s="639" t="s">
+      <c r="T75" s="638" t="s">
         <v>210</v>
       </c>
       <c r="U75" s="83" t="s">
@@ -13156,7 +13162,7 @@
       <c r="W75" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="Y75" s="639" t="s">
+      <c r="Y75" s="638" t="s">
         <v>210</v>
       </c>
       <c r="Z75" s="83" t="s">
@@ -13170,7 +13176,7 @@
       </c>
     </row>
     <row r="76" spans="2:28">
-      <c r="T76" s="641"/>
+      <c r="T76" s="639"/>
       <c r="U76" s="83" t="s">
         <v>212</v>
       </c>
@@ -13180,7 +13186,7 @@
       <c r="W76" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="Y76" s="641"/>
+      <c r="Y76" s="639"/>
       <c r="Z76" s="83" t="s">
         <v>212</v>
       </c>
@@ -13214,7 +13220,7 @@
       </c>
     </row>
     <row r="78" spans="2:28">
-      <c r="T78" s="639" t="s">
+      <c r="T78" s="638" t="s">
         <v>216</v>
       </c>
       <c r="U78" s="81" t="s">
@@ -13226,7 +13232,7 @@
       <c r="W78" s="100" t="s">
         <v>284</v>
       </c>
-      <c r="Y78" s="639" t="s">
+      <c r="Y78" s="638" t="s">
         <v>216</v>
       </c>
       <c r="Z78" s="81" t="s">
@@ -13262,7 +13268,7 @@
       </c>
     </row>
     <row r="80" spans="2:28">
-      <c r="T80" s="639" t="s">
+      <c r="T80" s="638" t="s">
         <v>225</v>
       </c>
       <c r="U80" s="364" t="s">
@@ -13274,7 +13280,7 @@
       <c r="W80" s="369" t="s">
         <v>238</v>
       </c>
-      <c r="Y80" s="639" t="s">
+      <c r="Y80" s="638" t="s">
         <v>225</v>
       </c>
       <c r="Z80" s="364" t="s">
@@ -13288,7 +13294,7 @@
       </c>
     </row>
     <row r="81" spans="20:28">
-      <c r="T81" s="641"/>
+      <c r="T81" s="639"/>
       <c r="U81" s="365" t="s">
         <v>228</v>
       </c>
@@ -13296,7 +13302,7 @@
         <v>229</v>
       </c>
       <c r="W81" s="370"/>
-      <c r="Y81" s="641"/>
+      <c r="Y81" s="639"/>
       <c r="Z81" s="365" t="s">
         <v>228</v>
       </c>
@@ -13328,7 +13334,7 @@
       </c>
     </row>
     <row r="83" spans="20:28">
-      <c r="T83" s="639" t="s">
+      <c r="T83" s="638" t="s">
         <v>236</v>
       </c>
       <c r="U83" s="82" t="s">
@@ -13340,7 +13346,7 @@
       <c r="W83" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="Y83" s="639" t="s">
+      <c r="Y83" s="638" t="s">
         <v>236</v>
       </c>
       <c r="Z83" s="82" t="s">
@@ -13354,7 +13360,7 @@
       </c>
     </row>
     <row r="84" spans="20:28" ht="16.5" thickBot="1">
-      <c r="T84" s="642"/>
+      <c r="T84" s="641"/>
       <c r="U84" s="89" t="s">
         <v>241</v>
       </c>
@@ -13364,7 +13370,7 @@
       <c r="W84" s="114" t="s">
         <v>292</v>
       </c>
-      <c r="Y84" s="642"/>
+      <c r="Y84" s="641"/>
       <c r="Z84" s="89" t="s">
         <v>241</v>
       </c>
@@ -13377,34 +13383,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="Y73:AB73"/>
-    <mergeCell ref="Y75:Y77"/>
-    <mergeCell ref="Y78:Y79"/>
-    <mergeCell ref="Y80:Y82"/>
-    <mergeCell ref="Y83:Y84"/>
-    <mergeCell ref="Y60:AB60"/>
-    <mergeCell ref="Y62:Y64"/>
-    <mergeCell ref="Y65:Y66"/>
-    <mergeCell ref="Y67:Y69"/>
-    <mergeCell ref="Y70:Y71"/>
-    <mergeCell ref="Y47:AB47"/>
-    <mergeCell ref="Y49:Y51"/>
-    <mergeCell ref="Y52:Y53"/>
-    <mergeCell ref="Y54:Y56"/>
-    <mergeCell ref="Y57:Y58"/>
-    <mergeCell ref="Y34:AB34"/>
-    <mergeCell ref="Y36:Y38"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="Y41:Y43"/>
-    <mergeCell ref="Y44:Y45"/>
-    <mergeCell ref="T80:T82"/>
-    <mergeCell ref="T83:T84"/>
-    <mergeCell ref="T75:T77"/>
-    <mergeCell ref="T78:T79"/>
-    <mergeCell ref="T65:T66"/>
-    <mergeCell ref="T73:W73"/>
-    <mergeCell ref="T70:T71"/>
-    <mergeCell ref="T67:T69"/>
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="T47:W47"/>
     <mergeCell ref="T60:W60"/>
@@ -13417,6 +13395,34 @@
     <mergeCell ref="T41:T43"/>
     <mergeCell ref="T44:T45"/>
     <mergeCell ref="T49:T51"/>
+    <mergeCell ref="T80:T82"/>
+    <mergeCell ref="T83:T84"/>
+    <mergeCell ref="T75:T77"/>
+    <mergeCell ref="T78:T79"/>
+    <mergeCell ref="T65:T66"/>
+    <mergeCell ref="T73:W73"/>
+    <mergeCell ref="T70:T71"/>
+    <mergeCell ref="T67:T69"/>
+    <mergeCell ref="Y34:AB34"/>
+    <mergeCell ref="Y36:Y38"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="Y41:Y43"/>
+    <mergeCell ref="Y44:Y45"/>
+    <mergeCell ref="Y47:AB47"/>
+    <mergeCell ref="Y49:Y51"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="Y54:Y56"/>
+    <mergeCell ref="Y57:Y58"/>
+    <mergeCell ref="Y60:AB60"/>
+    <mergeCell ref="Y62:Y64"/>
+    <mergeCell ref="Y65:Y66"/>
+    <mergeCell ref="Y67:Y69"/>
+    <mergeCell ref="Y70:Y71"/>
+    <mergeCell ref="Y73:AB73"/>
+    <mergeCell ref="Y75:Y77"/>
+    <mergeCell ref="Y78:Y79"/>
+    <mergeCell ref="Y80:Y82"/>
+    <mergeCell ref="Y83:Y84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" orientation="portrait" r:id="rId1"/>
@@ -13475,18 +13481,18 @@
       <c r="L2" s="202"/>
     </row>
     <row r="3" spans="2:12" ht="21">
-      <c r="B3" s="623" t="s">
+      <c r="B3" s="622" t="s">
         <v>294</v>
       </c>
-      <c r="C3" s="624"/>
-      <c r="D3" s="624"/>
-      <c r="E3" s="624"/>
-      <c r="F3" s="624"/>
-      <c r="G3" s="624"/>
-      <c r="H3" s="624"/>
-      <c r="I3" s="624"/>
-      <c r="J3" s="624"/>
-      <c r="K3" s="625"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
+      <c r="G3" s="623"/>
+      <c r="H3" s="623"/>
+      <c r="I3" s="623"/>
+      <c r="J3" s="623"/>
+      <c r="K3" s="624"/>
       <c r="L3" s="202"/>
     </row>
     <row r="4" spans="2:12" ht="63">
@@ -13771,14 +13777,14 @@
       <c r="L14" s="202"/>
     </row>
     <row r="15" spans="2:12" ht="21">
-      <c r="B15" s="626" t="s">
+      <c r="B15" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="627"/>
-      <c r="D15" s="627"/>
-      <c r="E15" s="627"/>
-      <c r="F15" s="627"/>
-      <c r="G15" s="627"/>
+      <c r="C15" s="626"/>
+      <c r="D15" s="626"/>
+      <c r="E15" s="626"/>
+      <c r="F15" s="626"/>
+      <c r="G15" s="626"/>
       <c r="H15" s="231">
         <f>SUM(H5:H14)</f>
         <v>7.8999999999999995</v>
@@ -13798,14 +13804,14 @@
       <c r="L15" s="202"/>
     </row>
     <row r="16" spans="2:12" ht="21">
-      <c r="B16" s="626" t="s">
+      <c r="B16" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C16" s="627"/>
-      <c r="D16" s="627"/>
-      <c r="E16" s="627"/>
-      <c r="F16" s="627"/>
-      <c r="G16" s="627"/>
+      <c r="C16" s="626"/>
+      <c r="D16" s="626"/>
+      <c r="E16" s="626"/>
+      <c r="F16" s="626"/>
+      <c r="G16" s="626"/>
       <c r="H16" s="231">
         <f>(20.5-H15)</f>
         <v>12.600000000000001</v>
@@ -13825,14 +13831,14 @@
       <c r="L16" s="202"/>
     </row>
     <row r="17" spans="2:17" ht="27" customHeight="1" thickBot="1">
-      <c r="B17" s="628" t="s">
+      <c r="B17" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="629"/>
-      <c r="D17" s="629"/>
-      <c r="E17" s="629"/>
-      <c r="F17" s="629"/>
-      <c r="G17" s="629"/>
+      <c r="C17" s="628"/>
+      <c r="D17" s="628"/>
+      <c r="E17" s="628"/>
+      <c r="F17" s="628"/>
+      <c r="G17" s="628"/>
       <c r="H17" s="312">
         <f>(H15+H16)-1</f>
         <v>19.5</v>
@@ -13860,19 +13866,19 @@
       <c r="L18" s="202"/>
     </row>
     <row r="19" spans="2:17" ht="21">
-      <c r="B19" s="644" t="s">
+      <c r="B19" s="643" t="s">
         <v>300</v>
       </c>
-      <c r="C19" s="645"/>
-      <c r="D19" s="645"/>
-      <c r="E19" s="645"/>
-      <c r="F19" s="645"/>
-      <c r="G19" s="645"/>
-      <c r="H19" s="645"/>
-      <c r="I19" s="645"/>
-      <c r="J19" s="645"/>
-      <c r="K19" s="645"/>
-      <c r="L19" s="646"/>
+      <c r="C19" s="644"/>
+      <c r="D19" s="644"/>
+      <c r="E19" s="644"/>
+      <c r="F19" s="644"/>
+      <c r="G19" s="644"/>
+      <c r="H19" s="644"/>
+      <c r="I19" s="644"/>
+      <c r="J19" s="644"/>
+      <c r="K19" s="644"/>
+      <c r="L19" s="645"/>
     </row>
     <row r="20" spans="2:17" ht="63">
       <c r="B20" s="288" t="s">
@@ -14160,14 +14166,14 @@
       <c r="L30" s="296"/>
     </row>
     <row r="31" spans="2:17" ht="21">
-      <c r="B31" s="626" t="s">
+      <c r="B31" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="627"/>
-      <c r="D31" s="627"/>
-      <c r="E31" s="627"/>
-      <c r="F31" s="627"/>
-      <c r="G31" s="627"/>
+      <c r="C31" s="626"/>
+      <c r="D31" s="626"/>
+      <c r="E31" s="626"/>
+      <c r="F31" s="626"/>
+      <c r="G31" s="626"/>
       <c r="H31" s="231">
         <f>SUM(H21:H30)</f>
         <v>8.6</v>
@@ -14190,14 +14196,14 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="21">
-      <c r="B32" s="626" t="s">
+      <c r="B32" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C32" s="627"/>
-      <c r="D32" s="627"/>
-      <c r="E32" s="627"/>
-      <c r="F32" s="627"/>
-      <c r="G32" s="627"/>
+      <c r="C32" s="626"/>
+      <c r="D32" s="626"/>
+      <c r="E32" s="626"/>
+      <c r="F32" s="626"/>
+      <c r="G32" s="626"/>
       <c r="H32" s="231">
         <f>20.5-H31</f>
         <v>11.9</v>
@@ -14220,14 +14226,14 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B33" s="628" t="s">
+      <c r="B33" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="629"/>
-      <c r="D33" s="629"/>
-      <c r="E33" s="629"/>
-      <c r="F33" s="629"/>
-      <c r="G33" s="629"/>
+      <c r="C33" s="628"/>
+      <c r="D33" s="628"/>
+      <c r="E33" s="628"/>
+      <c r="F33" s="628"/>
+      <c r="G33" s="628"/>
       <c r="H33" s="312">
         <f>(H31+H32)-1</f>
         <v>19.5</v>
@@ -14257,16 +14263,16 @@
       <c r="L34" s="202"/>
     </row>
     <row r="35" spans="2:12" ht="21">
-      <c r="B35" s="623" t="s">
+      <c r="B35" s="622" t="s">
         <v>305</v>
       </c>
-      <c r="C35" s="624"/>
-      <c r="D35" s="624"/>
-      <c r="E35" s="624"/>
-      <c r="F35" s="624"/>
-      <c r="G35" s="624"/>
-      <c r="H35" s="624"/>
-      <c r="I35" s="625"/>
+      <c r="C35" s="623"/>
+      <c r="D35" s="623"/>
+      <c r="E35" s="623"/>
+      <c r="F35" s="623"/>
+      <c r="G35" s="623"/>
+      <c r="H35" s="623"/>
+      <c r="I35" s="624"/>
       <c r="J35" s="202"/>
       <c r="K35" s="202"/>
       <c r="L35" s="202"/>
@@ -14558,14 +14564,14 @@
       <c r="L46" s="202"/>
     </row>
     <row r="47" spans="2:12" ht="21">
-      <c r="B47" s="626" t="s">
+      <c r="B47" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="627"/>
-      <c r="D47" s="627"/>
-      <c r="E47" s="627"/>
-      <c r="F47" s="627"/>
-      <c r="G47" s="627"/>
+      <c r="C47" s="626"/>
+      <c r="D47" s="626"/>
+      <c r="E47" s="626"/>
+      <c r="F47" s="626"/>
+      <c r="G47" s="626"/>
       <c r="H47" s="231">
         <f>SUM(H37:H46)</f>
         <v>13.5</v>
@@ -14579,14 +14585,14 @@
       <c r="L47" s="202"/>
     </row>
     <row r="48" spans="2:12" ht="21">
-      <c r="B48" s="626" t="s">
+      <c r="B48" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C48" s="627"/>
-      <c r="D48" s="627"/>
-      <c r="E48" s="627"/>
-      <c r="F48" s="627"/>
-      <c r="G48" s="627"/>
+      <c r="C48" s="626"/>
+      <c r="D48" s="626"/>
+      <c r="E48" s="626"/>
+      <c r="F48" s="626"/>
+      <c r="G48" s="626"/>
       <c r="H48" s="231">
         <f>20.5-H47</f>
         <v>7</v>
@@ -14600,14 +14606,14 @@
       <c r="L48" s="202"/>
     </row>
     <row r="49" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B49" s="628" t="s">
+      <c r="B49" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="629"/>
-      <c r="D49" s="629"/>
-      <c r="E49" s="629"/>
-      <c r="F49" s="629"/>
-      <c r="G49" s="629"/>
+      <c r="C49" s="628"/>
+      <c r="D49" s="628"/>
+      <c r="E49" s="628"/>
+      <c r="F49" s="628"/>
+      <c r="G49" s="628"/>
       <c r="H49" s="312">
         <f>(H47+H48)-1</f>
         <v>19.5</v>
@@ -14631,18 +14637,18 @@
       <c r="L50" s="202"/>
     </row>
     <row r="51" spans="2:12" ht="21">
-      <c r="B51" s="623" t="s">
+      <c r="B51" s="622" t="s">
         <v>306</v>
       </c>
-      <c r="C51" s="624"/>
-      <c r="D51" s="624"/>
-      <c r="E51" s="624"/>
-      <c r="F51" s="624"/>
-      <c r="G51" s="624"/>
-      <c r="H51" s="624"/>
-      <c r="I51" s="624"/>
-      <c r="J51" s="624"/>
-      <c r="K51" s="625"/>
+      <c r="C51" s="623"/>
+      <c r="D51" s="623"/>
+      <c r="E51" s="623"/>
+      <c r="F51" s="623"/>
+      <c r="G51" s="623"/>
+      <c r="H51" s="623"/>
+      <c r="I51" s="623"/>
+      <c r="J51" s="623"/>
+      <c r="K51" s="624"/>
       <c r="L51" s="202"/>
     </row>
     <row r="52" spans="2:12" ht="63">
@@ -14927,14 +14933,14 @@
       <c r="L62" s="202"/>
     </row>
     <row r="63" spans="2:12" ht="21">
-      <c r="B63" s="626" t="s">
+      <c r="B63" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="627"/>
-      <c r="D63" s="627"/>
-      <c r="E63" s="627"/>
-      <c r="F63" s="627"/>
-      <c r="G63" s="627"/>
+      <c r="C63" s="626"/>
+      <c r="D63" s="626"/>
+      <c r="E63" s="626"/>
+      <c r="F63" s="626"/>
+      <c r="G63" s="626"/>
       <c r="H63" s="231">
         <f>SUM(H53:H62)</f>
         <v>8.1999999999999993</v>
@@ -14954,14 +14960,14 @@
       <c r="L63" s="202"/>
     </row>
     <row r="64" spans="2:12" ht="21">
-      <c r="B64" s="626" t="s">
+      <c r="B64" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C64" s="627"/>
-      <c r="D64" s="627"/>
-      <c r="E64" s="627"/>
-      <c r="F64" s="627"/>
-      <c r="G64" s="627"/>
+      <c r="C64" s="626"/>
+      <c r="D64" s="626"/>
+      <c r="E64" s="626"/>
+      <c r="F64" s="626"/>
+      <c r="G64" s="626"/>
       <c r="H64" s="231">
         <f>20.5-H63</f>
         <v>12.3</v>
@@ -14981,14 +14987,14 @@
       <c r="L64" s="202"/>
     </row>
     <row r="65" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B65" s="628" t="s">
+      <c r="B65" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C65" s="629"/>
-      <c r="D65" s="629"/>
-      <c r="E65" s="629"/>
-      <c r="F65" s="629"/>
-      <c r="G65" s="629"/>
+      <c r="C65" s="628"/>
+      <c r="D65" s="628"/>
+      <c r="E65" s="628"/>
+      <c r="F65" s="628"/>
+      <c r="G65" s="628"/>
       <c r="H65" s="312">
         <f>(H63+H64)-1</f>
         <v>19.5</v>
@@ -15003,12 +15009,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B16:G16"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B63:G63"/>
     <mergeCell ref="B64:G64"/>
@@ -15019,6 +15019,12 @@
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B35:I35"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
@@ -15078,18 +15084,18 @@
       <c r="L2" s="202"/>
     </row>
     <row r="3" spans="2:12" ht="21">
-      <c r="B3" s="623" t="s">
+      <c r="B3" s="622" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="624"/>
-      <c r="D3" s="624"/>
-      <c r="E3" s="624"/>
-      <c r="F3" s="624"/>
-      <c r="G3" s="624"/>
-      <c r="H3" s="624"/>
-      <c r="I3" s="624"/>
-      <c r="J3" s="624"/>
-      <c r="K3" s="625"/>
+      <c r="C3" s="623"/>
+      <c r="D3" s="623"/>
+      <c r="E3" s="623"/>
+      <c r="F3" s="623"/>
+      <c r="G3" s="623"/>
+      <c r="H3" s="623"/>
+      <c r="I3" s="623"/>
+      <c r="J3" s="623"/>
+      <c r="K3" s="624"/>
       <c r="L3" s="202"/>
     </row>
     <row r="4" spans="2:12" ht="63">
@@ -15367,14 +15373,14 @@
       <c r="L14" s="202"/>
     </row>
     <row r="15" spans="2:12" ht="21">
-      <c r="B15" s="626" t="s">
+      <c r="B15" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="627"/>
-      <c r="D15" s="627"/>
-      <c r="E15" s="627"/>
-      <c r="F15" s="627"/>
-      <c r="G15" s="627"/>
+      <c r="C15" s="626"/>
+      <c r="D15" s="626"/>
+      <c r="E15" s="626"/>
+      <c r="F15" s="626"/>
+      <c r="G15" s="626"/>
       <c r="H15" s="189">
         <f>SUM(H5:H14)</f>
         <v>8.3999999999999986</v>
@@ -15394,14 +15400,14 @@
       <c r="L15" s="202"/>
     </row>
     <row r="16" spans="2:12" ht="21">
-      <c r="B16" s="626" t="s">
+      <c r="B16" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C16" s="627"/>
-      <c r="D16" s="627"/>
-      <c r="E16" s="627"/>
-      <c r="F16" s="627"/>
-      <c r="G16" s="627"/>
+      <c r="C16" s="626"/>
+      <c r="D16" s="626"/>
+      <c r="E16" s="626"/>
+      <c r="F16" s="626"/>
+      <c r="G16" s="626"/>
       <c r="H16" s="189">
         <f>(20.5-H15)</f>
         <v>12.100000000000001</v>
@@ -15421,14 +15427,14 @@
       <c r="L16" s="202"/>
     </row>
     <row r="17" spans="2:17" ht="27" customHeight="1" thickBot="1">
-      <c r="B17" s="628" t="s">
+      <c r="B17" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="629"/>
-      <c r="D17" s="629"/>
-      <c r="E17" s="629"/>
-      <c r="F17" s="629"/>
-      <c r="G17" s="629"/>
+      <c r="C17" s="628"/>
+      <c r="D17" s="628"/>
+      <c r="E17" s="628"/>
+      <c r="F17" s="628"/>
+      <c r="G17" s="628"/>
       <c r="H17" s="348">
         <f>(H15+H16)-1</f>
         <v>19.5</v>
@@ -15456,19 +15462,19 @@
       <c r="L18" s="202"/>
     </row>
     <row r="19" spans="2:17" ht="21">
-      <c r="B19" s="644" t="s">
+      <c r="B19" s="643" t="s">
         <v>313</v>
       </c>
-      <c r="C19" s="645"/>
-      <c r="D19" s="645"/>
-      <c r="E19" s="645"/>
-      <c r="F19" s="645"/>
-      <c r="G19" s="645"/>
-      <c r="H19" s="645"/>
-      <c r="I19" s="645"/>
-      <c r="J19" s="645"/>
-      <c r="K19" s="645"/>
-      <c r="L19" s="646"/>
+      <c r="C19" s="644"/>
+      <c r="D19" s="644"/>
+      <c r="E19" s="644"/>
+      <c r="F19" s="644"/>
+      <c r="G19" s="644"/>
+      <c r="H19" s="644"/>
+      <c r="I19" s="644"/>
+      <c r="J19" s="644"/>
+      <c r="K19" s="644"/>
+      <c r="L19" s="645"/>
     </row>
     <row r="20" spans="2:17" ht="63">
       <c r="B20" s="288" t="s">
@@ -15756,14 +15762,14 @@
       <c r="L30" s="335"/>
     </row>
     <row r="31" spans="2:17" ht="21">
-      <c r="B31" s="626" t="s">
+      <c r="B31" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="627"/>
-      <c r="D31" s="627"/>
-      <c r="E31" s="627"/>
-      <c r="F31" s="627"/>
-      <c r="G31" s="627"/>
+      <c r="C31" s="626"/>
+      <c r="D31" s="626"/>
+      <c r="E31" s="626"/>
+      <c r="F31" s="626"/>
+      <c r="G31" s="626"/>
       <c r="H31" s="189">
         <f>SUM(H21:H30)</f>
         <v>8.6</v>
@@ -15786,14 +15792,14 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="21">
-      <c r="B32" s="626" t="s">
+      <c r="B32" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C32" s="627"/>
-      <c r="D32" s="627"/>
-      <c r="E32" s="627"/>
-      <c r="F32" s="627"/>
-      <c r="G32" s="627"/>
+      <c r="C32" s="626"/>
+      <c r="D32" s="626"/>
+      <c r="E32" s="626"/>
+      <c r="F32" s="626"/>
+      <c r="G32" s="626"/>
       <c r="H32" s="189">
         <f>20.5-H31</f>
         <v>11.9</v>
@@ -15816,14 +15822,14 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B33" s="628" t="s">
+      <c r="B33" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="629"/>
-      <c r="D33" s="629"/>
-      <c r="E33" s="629"/>
-      <c r="F33" s="629"/>
-      <c r="G33" s="629"/>
+      <c r="C33" s="628"/>
+      <c r="D33" s="628"/>
+      <c r="E33" s="628"/>
+      <c r="F33" s="628"/>
+      <c r="G33" s="628"/>
       <c r="H33" s="348">
         <f>(H31+H32)-1</f>
         <v>19.5</v>
@@ -15853,16 +15859,16 @@
       <c r="L34" s="202"/>
     </row>
     <row r="35" spans="2:12" ht="21">
-      <c r="B35" s="623" t="s">
+      <c r="B35" s="622" t="s">
         <v>314</v>
       </c>
-      <c r="C35" s="624"/>
-      <c r="D35" s="624"/>
-      <c r="E35" s="624"/>
-      <c r="F35" s="624"/>
-      <c r="G35" s="624"/>
-      <c r="H35" s="624"/>
-      <c r="I35" s="625"/>
+      <c r="C35" s="623"/>
+      <c r="D35" s="623"/>
+      <c r="E35" s="623"/>
+      <c r="F35" s="623"/>
+      <c r="G35" s="623"/>
+      <c r="H35" s="623"/>
+      <c r="I35" s="624"/>
       <c r="J35" s="202"/>
       <c r="K35" s="202"/>
       <c r="L35" s="202"/>
@@ -16154,14 +16160,14 @@
       <c r="L46" s="202"/>
     </row>
     <row r="47" spans="2:12" ht="21">
-      <c r="B47" s="626" t="s">
+      <c r="B47" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="627"/>
-      <c r="D47" s="627"/>
-      <c r="E47" s="627"/>
-      <c r="F47" s="627"/>
-      <c r="G47" s="627"/>
+      <c r="C47" s="626"/>
+      <c r="D47" s="626"/>
+      <c r="E47" s="626"/>
+      <c r="F47" s="626"/>
+      <c r="G47" s="626"/>
       <c r="H47" s="189">
         <f>SUM(H37:H46)</f>
         <v>14.5</v>
@@ -16175,14 +16181,14 @@
       <c r="L47" s="202"/>
     </row>
     <row r="48" spans="2:12" ht="21">
-      <c r="B48" s="626" t="s">
+      <c r="B48" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C48" s="627"/>
-      <c r="D48" s="627"/>
-      <c r="E48" s="627"/>
-      <c r="F48" s="627"/>
-      <c r="G48" s="627"/>
+      <c r="C48" s="626"/>
+      <c r="D48" s="626"/>
+      <c r="E48" s="626"/>
+      <c r="F48" s="626"/>
+      <c r="G48" s="626"/>
       <c r="H48" s="189">
         <f>20.5-H47</f>
         <v>6</v>
@@ -16196,14 +16202,14 @@
       <c r="L48" s="202"/>
     </row>
     <row r="49" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B49" s="628" t="s">
+      <c r="B49" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="629"/>
-      <c r="D49" s="629"/>
-      <c r="E49" s="629"/>
-      <c r="F49" s="629"/>
-      <c r="G49" s="629"/>
+      <c r="C49" s="628"/>
+      <c r="D49" s="628"/>
+      <c r="E49" s="628"/>
+      <c r="F49" s="628"/>
+      <c r="G49" s="628"/>
       <c r="H49" s="348">
         <f>(H47+H48)-1</f>
         <v>19.5</v>
@@ -16227,18 +16233,18 @@
       <c r="L50" s="202"/>
     </row>
     <row r="51" spans="2:12" ht="21.75">
-      <c r="B51" s="623" t="s">
+      <c r="B51" s="622" t="s">
         <v>315</v>
       </c>
-      <c r="C51" s="624"/>
-      <c r="D51" s="624"/>
-      <c r="E51" s="624"/>
-      <c r="F51" s="624"/>
-      <c r="G51" s="624"/>
-      <c r="H51" s="624"/>
-      <c r="I51" s="624"/>
-      <c r="J51" s="624"/>
-      <c r="K51" s="625"/>
+      <c r="C51" s="623"/>
+      <c r="D51" s="623"/>
+      <c r="E51" s="623"/>
+      <c r="F51" s="623"/>
+      <c r="G51" s="623"/>
+      <c r="H51" s="623"/>
+      <c r="I51" s="623"/>
+      <c r="J51" s="623"/>
+      <c r="K51" s="624"/>
       <c r="L51" s="202"/>
     </row>
     <row r="52" spans="2:12" ht="63">
@@ -16363,13 +16369,13 @@
         <v>284</v>
       </c>
       <c r="F56" s="238"/>
-      <c r="G56" s="647" t="s">
+      <c r="G56" s="646" t="s">
         <v>316</v>
       </c>
-      <c r="H56" s="648"/>
-      <c r="I56" s="648"/>
-      <c r="J56" s="648"/>
-      <c r="K56" s="649"/>
+      <c r="H56" s="647"/>
+      <c r="I56" s="647"/>
+      <c r="J56" s="647"/>
+      <c r="K56" s="648"/>
       <c r="L56" s="202"/>
     </row>
     <row r="57" spans="2:12" ht="21.75">
@@ -16523,14 +16529,14 @@
       <c r="L62" s="202"/>
     </row>
     <row r="63" spans="2:12" ht="21">
-      <c r="B63" s="626" t="s">
+      <c r="B63" s="625" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="627"/>
-      <c r="D63" s="627"/>
-      <c r="E63" s="627"/>
-      <c r="F63" s="627"/>
-      <c r="G63" s="627"/>
+      <c r="C63" s="626"/>
+      <c r="D63" s="626"/>
+      <c r="E63" s="626"/>
+      <c r="F63" s="626"/>
+      <c r="G63" s="626"/>
       <c r="H63" s="189">
         <f>SUM(H53:H62)</f>
         <v>8.8000000000000007</v>
@@ -16550,14 +16556,14 @@
       <c r="L63" s="202"/>
     </row>
     <row r="64" spans="2:12" ht="21">
-      <c r="B64" s="626" t="s">
+      <c r="B64" s="625" t="s">
         <v>299</v>
       </c>
-      <c r="C64" s="627"/>
-      <c r="D64" s="627"/>
-      <c r="E64" s="627"/>
-      <c r="F64" s="627"/>
-      <c r="G64" s="627"/>
+      <c r="C64" s="626"/>
+      <c r="D64" s="626"/>
+      <c r="E64" s="626"/>
+      <c r="F64" s="626"/>
+      <c r="G64" s="626"/>
       <c r="H64" s="189">
         <f>20.5-H63</f>
         <v>11.7</v>
@@ -16577,14 +16583,14 @@
       <c r="L64" s="202"/>
     </row>
     <row r="65" spans="2:12" ht="21.75" thickBot="1">
-      <c r="B65" s="628" t="s">
+      <c r="B65" s="627" t="s">
         <v>54</v>
       </c>
-      <c r="C65" s="629"/>
-      <c r="D65" s="629"/>
-      <c r="E65" s="629"/>
-      <c r="F65" s="629"/>
-      <c r="G65" s="629"/>
+      <c r="C65" s="628"/>
+      <c r="D65" s="628"/>
+      <c r="E65" s="628"/>
+      <c r="F65" s="628"/>
+      <c r="G65" s="628"/>
       <c r="H65" s="348">
         <f>(H63+H64)-1</f>
         <v>19.5</v>
@@ -16599,6 +16605,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="G56:K56"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B15:G15"/>
@@ -16611,11 +16622,6 @@
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="G56:K56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
@@ -16630,10 +16636,10 @@
   <dimension ref="B1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD15" sqref="AD15"/>
+      <selection pane="bottomRight" sqref="A1:W60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -16673,10 +16679,10 @@
       <c r="H1" s="400" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="618" t="s">
+      <c r="Q1" s="617" t="s">
         <v>317</v>
       </c>
-      <c r="R1" s="618"/>
+      <c r="R1" s="617"/>
       <c r="S1" s="400"/>
     </row>
     <row r="2" spans="2:25" ht="90.75" customHeight="1">
@@ -16702,7 +16708,7 @@
         <v>62</v>
       </c>
       <c r="I2" s="418">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="J2" s="421" t="s">
         <v>318</v>
@@ -16714,13 +16720,13 @@
         <v>359</v>
       </c>
       <c r="M2" s="418">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N2" s="423" t="s">
         <v>66</v>
       </c>
       <c r="O2" s="419">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P2" s="424" t="s">
         <v>320</v>
@@ -16732,7 +16738,7 @@
         <v>321</v>
       </c>
       <c r="S2" s="425">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="X2" s="405"/>
       <c r="Y2" s="405"/>
@@ -16796,14 +16802,14 @@
       </c>
       <c r="O4" s="433">
         <f>N4*O2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="P4" s="434"/>
       <c r="Q4" s="435"/>
       <c r="R4" s="427"/>
       <c r="S4" s="464"/>
       <c r="U4" s="512" t="s">
-        <v>99</v>
+        <v>418</v>
       </c>
       <c r="V4" s="508"/>
       <c r="W4" s="401"/>
@@ -16834,7 +16840,7 @@
       <c r="R5" s="427"/>
       <c r="S5" s="464"/>
       <c r="U5" s="512" t="s">
-        <v>102</v>
+        <v>419</v>
       </c>
       <c r="V5" s="508"/>
       <c r="W5" s="401"/>
@@ -16907,7 +16913,7 @@
       </c>
       <c r="S7" s="436">
         <f>R7*S2</f>
-        <v>23.200000000000003</v>
+        <v>19.200000000000003</v>
       </c>
       <c r="T7" s="380"/>
       <c r="U7" s="508"/>
@@ -16944,7 +16950,7 @@
       </c>
       <c r="M8" s="519">
         <f>M2*L8</f>
-        <v>52.2</v>
+        <v>43.2</v>
       </c>
       <c r="N8" s="449"/>
       <c r="O8" s="450"/>
@@ -16991,7 +16997,7 @@
       </c>
       <c r="O9" s="433">
         <f>N9*O2</f>
-        <v>14.5</v>
+        <v>12</v>
       </c>
       <c r="P9" s="434"/>
       <c r="Q9" s="443"/>
@@ -17000,7 +17006,7 @@
       </c>
       <c r="S9" s="436">
         <f>R9*S2</f>
-        <v>2.9000000000000004</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="T9" s="380"/>
       <c r="W9" s="401"/>
@@ -17035,7 +17041,7 @@
       </c>
       <c r="O10" s="519">
         <f>O2*N10</f>
-        <v>14.5</v>
+        <v>12</v>
       </c>
       <c r="P10" s="434"/>
       <c r="Q10" s="435"/>
@@ -17078,7 +17084,7 @@
       </c>
       <c r="M11" s="494">
         <f>M2*L11</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="N11" s="449"/>
       <c r="O11" s="450"/>
@@ -17089,7 +17095,7 @@
       </c>
       <c r="S11" s="436">
         <f>R11*S2</f>
-        <v>5.8000000000000007</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="T11" s="380"/>
       <c r="U11" s="512" t="s">
@@ -17190,7 +17196,7 @@
       </c>
       <c r="O14" s="433">
         <f>N14*O2</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="P14" s="434"/>
       <c r="Q14" s="443"/>
@@ -17231,7 +17237,7 @@
       </c>
       <c r="O15" s="433">
         <f>N15*O2</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="P15" s="434"/>
       <c r="Q15" s="443"/>
@@ -17304,7 +17310,7 @@
       </c>
       <c r="M17" s="518">
         <f>M2*L17</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="N17" s="604"/>
       <c r="O17" s="450"/>
@@ -17408,12 +17414,12 @@
       <c r="K20" s="430"/>
       <c r="L20" s="430"/>
       <c r="M20" s="430"/>
-      <c r="N20" s="616">
-        <v>0.9</v>
+      <c r="N20" s="442">
+        <v>0.8</v>
       </c>
       <c r="O20" s="519">
         <f>O2*N20</f>
-        <v>26.1</v>
+        <v>19.200000000000003</v>
       </c>
       <c r="P20" s="434"/>
       <c r="Q20" s="435"/>
@@ -17451,7 +17457,7 @@
       <c r="S21" s="464"/>
       <c r="T21" s="380"/>
       <c r="U21" s="512" t="s">
-        <v>365</v>
+        <v>420</v>
       </c>
       <c r="V21" s="508"/>
       <c r="W21" s="402"/>
@@ -17483,12 +17489,12 @@
       <c r="K22" s="430"/>
       <c r="L22" s="427"/>
       <c r="M22" s="520"/>
-      <c r="N22" s="616">
+      <c r="N22" s="442">
         <v>0.9</v>
       </c>
       <c r="O22" s="519">
         <f>O2*N22</f>
-        <v>26.1</v>
+        <v>21.6</v>
       </c>
       <c r="P22" s="434"/>
       <c r="Q22" s="435"/>
@@ -17526,12 +17532,12 @@
       <c r="K23" s="451"/>
       <c r="L23" s="451"/>
       <c r="M23" s="451"/>
-      <c r="N23" s="616">
+      <c r="N23" s="442">
         <v>1</v>
       </c>
       <c r="O23" s="519">
         <f>O2*N23</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P23" s="434"/>
       <c r="Q23" s="435"/>
@@ -17572,7 +17578,7 @@
       </c>
       <c r="O24" s="553">
         <f>N24*O2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="P24" s="434"/>
       <c r="Q24" s="435"/>
@@ -17619,7 +17625,7 @@
       </c>
       <c r="S25" s="436">
         <f>R25*S2</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="T25" s="380"/>
       <c r="U25" s="512"/>
@@ -17656,7 +17662,7 @@
       </c>
       <c r="M26" s="494">
         <f>M2*L26</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="N26" s="449"/>
       <c r="O26" s="450"/>
@@ -17739,7 +17745,7 @@
       </c>
       <c r="S28" s="436">
         <f>R28*S2</f>
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="T28" s="380"/>
       <c r="U28" s="512"/>
@@ -17778,7 +17784,7 @@
       </c>
       <c r="O29" s="433">
         <f>N29*O2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="P29" s="434"/>
       <c r="Q29" s="435"/>
@@ -17787,7 +17793,7 @@
       </c>
       <c r="S29" s="436">
         <f>R29*S2</f>
-        <v>5.8000000000000007</v>
+        <v>4.8000000000000007</v>
       </c>
       <c r="T29" s="380"/>
       <c r="U29" s="512" t="s">
@@ -17828,7 +17834,7 @@
       </c>
       <c r="O30" s="519">
         <f>O2*N30</f>
-        <v>17.399999999999999</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="P30" s="434"/>
       <c r="Q30" s="435"/>
@@ -17867,7 +17873,7 @@
       </c>
       <c r="M31" s="518">
         <f>L31*M2</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N31" s="552"/>
       <c r="O31" s="450"/>
@@ -18008,7 +18014,7 @@
       </c>
       <c r="O35" s="519">
         <f>N35*O2</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P35" s="434"/>
       <c r="Q35" s="443"/>
@@ -18114,7 +18120,7 @@
       </c>
       <c r="O38" s="519">
         <f>N38*O2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="P38" s="434"/>
       <c r="Q38" s="443"/>
@@ -18158,10 +18164,12 @@
       <c r="O39" s="450"/>
       <c r="P39" s="434"/>
       <c r="Q39" s="435"/>
-      <c r="R39" s="617">
+      <c r="R39" s="616">
         <v>1.5</v>
       </c>
-      <c r="S39" s="599"/>
+      <c r="S39" s="599">
+        <v>1.5</v>
+      </c>
       <c r="T39" s="380"/>
       <c r="X39" s="405"/>
       <c r="Y39" s="405"/>
@@ -18227,7 +18235,7 @@
       </c>
       <c r="S41" s="436">
         <f>R41*S2</f>
-        <v>26.1</v>
+        <v>21.6</v>
       </c>
       <c r="T41" s="380"/>
       <c r="X41" s="405"/>
@@ -18286,7 +18294,7 @@
       </c>
       <c r="M43" s="518">
         <f>L43*M2</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N43" s="552"/>
       <c r="O43" s="450"/>
@@ -18353,7 +18361,7 @@
       </c>
       <c r="O45" s="519">
         <f>O2*N45</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="P45" s="434"/>
       <c r="Q45" s="435"/>
@@ -18389,7 +18397,7 @@
       </c>
       <c r="M46" s="519">
         <f>L46*M2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="N46" s="449"/>
       <c r="O46" s="450"/>
@@ -18431,7 +18439,7 @@
       </c>
       <c r="O47" s="433">
         <f>N47*O2</f>
-        <v>17.399999999999999</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="P47" s="434"/>
       <c r="Q47" s="435"/>
@@ -18496,7 +18504,7 @@
       </c>
       <c r="M49" s="494">
         <f>L49*M2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="N49" s="435"/>
       <c r="O49" s="450"/>
@@ -18542,7 +18550,7 @@
       </c>
       <c r="S50" s="436">
         <f>R50*S2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="T50" s="380"/>
       <c r="X50" s="405"/>
@@ -18599,7 +18607,7 @@
       </c>
       <c r="I52" s="452">
         <f>H52*I2</f>
-        <v>34.799999999999997</v>
+        <v>28.799999999999997</v>
       </c>
       <c r="J52" s="427"/>
       <c r="K52" s="471"/>
@@ -18706,7 +18714,7 @@
       </c>
       <c r="O55" s="433">
         <f>N55*O2</f>
-        <v>43.5</v>
+        <v>36</v>
       </c>
       <c r="P55" s="434"/>
       <c r="Q55" s="435"/>
@@ -18742,7 +18750,7 @@
       </c>
       <c r="M56" s="554">
         <f>L56*M2</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N56" s="530"/>
       <c r="O56" s="503"/>
@@ -18761,10 +18769,10 @@
       </c>
       <c r="D57" s="482"/>
       <c r="E57" s="483"/>
-      <c r="F57" s="619" t="s">
+      <c r="F57" s="618" t="s">
         <v>194</v>
       </c>
-      <c r="G57" s="619"/>
+      <c r="G57" s="618"/>
       <c r="H57" s="484">
         <f>SUM(H4:H56)</f>
         <v>1.2</v>
@@ -18780,15 +18788,15 @@
       </c>
       <c r="M57" s="556">
         <f>L57*M2</f>
-        <v>330.59999999999997</v>
+        <v>273.59999999999997</v>
       </c>
       <c r="N57" s="485">
         <f>SUM(N4:N56)</f>
-        <v>16.799999999999997</v>
+        <v>16.699999999999996</v>
       </c>
       <c r="O57" s="486">
         <f>N57*O2</f>
-        <v>487.19999999999993</v>
+        <v>400.7999999999999</v>
       </c>
       <c r="P57" s="487"/>
       <c r="Q57" s="488"/>
@@ -18798,7 +18806,7 @@
       </c>
       <c r="S57" s="490">
         <f>R57*S2</f>
-        <v>272.59999999999997</v>
+        <v>225.59999999999997</v>
       </c>
       <c r="Z57" s="381"/>
       <c r="AA57" s="403"/>
@@ -18810,10 +18818,10 @@
       <c r="C58" s="492"/>
       <c r="D58" s="549"/>
       <c r="E58" s="550"/>
-      <c r="F58" s="620" t="s">
+      <c r="F58" s="619" t="s">
         <v>196</v>
       </c>
-      <c r="G58" s="620"/>
+      <c r="G58" s="619"/>
       <c r="H58" s="493">
         <f>SUM(20.5-H57)</f>
         <v>19.3</v>
@@ -18829,15 +18837,15 @@
       </c>
       <c r="M58" s="555">
         <f>L58*M2</f>
-        <v>661.19999999999993</v>
+        <v>547.19999999999993</v>
       </c>
       <c r="N58" s="427">
         <f>N57*2</f>
-        <v>33.599999999999994</v>
+        <v>33.399999999999991</v>
       </c>
       <c r="O58" s="494">
         <f>N58*O2</f>
-        <v>974.39999999999986</v>
+        <v>801.5999999999998</v>
       </c>
       <c r="P58" s="439"/>
       <c r="Q58" s="495"/>
@@ -18847,7 +18855,7 @@
       </c>
       <c r="S58" s="436">
         <f>R58*S2</f>
-        <v>545.19999999999993</v>
+        <v>451.19999999999993</v>
       </c>
       <c r="T58" s="380"/>
       <c r="X58" s="403"/>
@@ -18860,19 +18868,19 @@
       <c r="C59" s="497"/>
       <c r="D59" s="498"/>
       <c r="E59" s="499"/>
-      <c r="F59" s="621" t="s">
+      <c r="F59" s="620" t="s">
         <v>198</v>
       </c>
-      <c r="G59" s="621"/>
+      <c r="G59" s="620"/>
       <c r="H59" s="500">
         <f>(H57+H58)-1</f>
         <v>19.5</v>
       </c>
       <c r="I59" s="474"/>
-      <c r="J59" s="622" t="s">
+      <c r="J59" s="621" t="s">
         <v>198</v>
       </c>
-      <c r="K59" s="622"/>
+      <c r="K59" s="621"/>
       <c r="L59" s="527">
         <f>(L57+L58)-3</f>
         <v>31.199999999999996</v>
@@ -18880,7 +18888,7 @@
       <c r="M59" s="523"/>
       <c r="N59" s="501">
         <f>(N57+N58)-3</f>
-        <v>47.399999999999991</v>
+        <v>47.099999999999987</v>
       </c>
       <c r="O59" s="502"/>
       <c r="P59" s="503"/>

</xml_diff>

<commit_message>
Antibody sheet for tomorrow's mix.
</commit_message>
<xml_diff>
--- a/2025_SFC_Panels.xlsx
+++ b/2025_SFC_Panels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drach\Documents\AlphaBeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A9BBA-5C4E-453B-A519-873665C605CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EE089F-3A85-48E8-9FCB-8C651E6861F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1646,9 +1646,6 @@
     <t>&lt;0.8&gt;</t>
   </si>
   <si>
-    <t>July 29th, 2025</t>
-  </si>
-  <si>
     <t>Wash with 1 ml PBS, spin down 1300rpm 8min</t>
   </si>
   <si>
@@ -1656,6 +1653,9 @@
   </si>
   <si>
     <t>0.75 ml Nuclear FixPerm, incubate @ 4C for  30min</t>
+  </si>
+  <si>
+    <t>July 31st, 2025</t>
   </si>
 </sst>
 </file>
@@ -4848,22 +4848,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -10972,19 +10972,19 @@
       <c r="R34" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="T34" s="642" t="s">
+      <c r="T34" s="637" t="s">
         <v>205</v>
       </c>
-      <c r="U34" s="642"/>
-      <c r="V34" s="642"/>
-      <c r="W34" s="642"/>
+      <c r="U34" s="637"/>
+      <c r="V34" s="637"/>
+      <c r="W34" s="637"/>
       <c r="X34" s="87"/>
-      <c r="Y34" s="642" t="s">
+      <c r="Y34" s="637" t="s">
         <v>206</v>
       </c>
-      <c r="Z34" s="642"/>
-      <c r="AA34" s="642"/>
-      <c r="AB34" s="642"/>
+      <c r="Z34" s="637"/>
+      <c r="AA34" s="637"/>
+      <c r="AB34" s="637"/>
       <c r="AH34" s="87"/>
     </row>
     <row r="35" spans="2:34">
@@ -11165,7 +11165,7 @@
         <v>9</v>
       </c>
       <c r="R37" s="145"/>
-      <c r="T37" s="639"/>
+      <c r="T37" s="640"/>
       <c r="U37" s="363" t="s">
         <v>212</v>
       </c>
@@ -11176,7 +11176,7 @@
         <v>44</v>
       </c>
       <c r="X37" s="87"/>
-      <c r="Y37" s="639"/>
+      <c r="Y37" s="640"/>
       <c r="Z37" s="363" t="s">
         <v>212</v>
       </c>
@@ -11236,7 +11236,7 @@
       <c r="R38" s="103" t="s">
         <v>214</v>
       </c>
-      <c r="T38" s="640"/>
+      <c r="T38" s="639"/>
       <c r="U38" s="363" t="s">
         <v>215</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>124</v>
       </c>
       <c r="X38" s="87"/>
-      <c r="Y38" s="640"/>
+      <c r="Y38" s="639"/>
       <c r="Z38" s="363" t="s">
         <v>215</v>
       </c>
@@ -11368,7 +11368,7 @@
       <c r="R40" s="103" t="s">
         <v>221</v>
       </c>
-      <c r="T40" s="640"/>
+      <c r="T40" s="639"/>
       <c r="U40" s="81" t="s">
         <v>222</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>29</v>
       </c>
       <c r="X40" s="87"/>
-      <c r="Y40" s="640"/>
+      <c r="Y40" s="639"/>
       <c r="Z40" s="81" t="s">
         <v>222</v>
       </c>
@@ -11502,7 +11502,7 @@
       <c r="R42" s="108" t="s">
         <v>108</v>
       </c>
-      <c r="T42" s="639"/>
+      <c r="T42" s="640"/>
       <c r="U42" s="365" t="s">
         <v>228</v>
       </c>
@@ -11511,7 +11511,7 @@
       </c>
       <c r="W42" s="370"/>
       <c r="X42" s="87"/>
-      <c r="Y42" s="639"/>
+      <c r="Y42" s="640"/>
       <c r="Z42" s="365" t="s">
         <v>228</v>
       </c>
@@ -11563,7 +11563,7 @@
       <c r="R43" s="162" t="s">
         <v>231</v>
       </c>
-      <c r="T43" s="640"/>
+      <c r="T43" s="639"/>
       <c r="U43" s="364" t="s">
         <v>232</v>
       </c>
@@ -11574,7 +11574,7 @@
         <v>233</v>
       </c>
       <c r="X43" s="87"/>
-      <c r="Y43" s="640"/>
+      <c r="Y43" s="639"/>
       <c r="Z43" s="364" t="s">
         <v>232</v>
       </c>
@@ -11807,19 +11807,19 @@
       <c r="R47" s="135" t="s">
         <v>245</v>
       </c>
-      <c r="T47" s="642" t="s">
+      <c r="T47" s="637" t="s">
         <v>246</v>
       </c>
-      <c r="U47" s="642"/>
-      <c r="V47" s="642"/>
-      <c r="W47" s="642"/>
+      <c r="U47" s="637"/>
+      <c r="V47" s="637"/>
+      <c r="W47" s="637"/>
       <c r="X47" s="87"/>
-      <c r="Y47" s="642" t="s">
+      <c r="Y47" s="637" t="s">
         <v>247</v>
       </c>
-      <c r="Z47" s="642"/>
-      <c r="AA47" s="642"/>
-      <c r="AB47" s="642"/>
+      <c r="Z47" s="637"/>
+      <c r="AA47" s="637"/>
+      <c r="AB47" s="637"/>
     </row>
     <row r="48" spans="2:34">
       <c r="B48" s="150"/>
@@ -11999,7 +11999,7 @@
       <c r="R50" s="103" t="s">
         <v>252</v>
       </c>
-      <c r="T50" s="639"/>
+      <c r="T50" s="640"/>
       <c r="U50" s="83" t="s">
         <v>212</v>
       </c>
@@ -12010,7 +12010,7 @@
         <v>29</v>
       </c>
       <c r="X50" s="87"/>
-      <c r="Y50" s="639"/>
+      <c r="Y50" s="640"/>
       <c r="Z50" s="83" t="s">
         <v>212</v>
       </c>
@@ -12061,7 +12061,7 @@
         <v>133</v>
       </c>
       <c r="R51" s="161"/>
-      <c r="T51" s="640"/>
+      <c r="T51" s="639"/>
       <c r="U51" s="83" t="s">
         <v>215</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>35</v>
       </c>
       <c r="X51" s="87"/>
-      <c r="Y51" s="640"/>
+      <c r="Y51" s="639"/>
       <c r="Z51" s="83" t="s">
         <v>215</v>
       </c>
@@ -12193,7 +12193,7 @@
       <c r="R53" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="T53" s="640"/>
+      <c r="T53" s="639"/>
       <c r="U53" s="81" t="s">
         <v>222</v>
       </c>
@@ -12204,7 +12204,7 @@
         <v>124</v>
       </c>
       <c r="X53" s="87"/>
-      <c r="Y53" s="640"/>
+      <c r="Y53" s="639"/>
       <c r="Z53" s="81" t="s">
         <v>222</v>
       </c>
@@ -12325,7 +12325,7 @@
       <c r="R55" s="135" t="s">
         <v>264</v>
       </c>
-      <c r="T55" s="639"/>
+      <c r="T55" s="640"/>
       <c r="U55" s="365" t="s">
         <v>228</v>
       </c>
@@ -12334,7 +12334,7 @@
       </c>
       <c r="W55" s="370"/>
       <c r="X55" s="87"/>
-      <c r="Y55" s="639"/>
+      <c r="Y55" s="640"/>
       <c r="Z55" s="365" t="s">
         <v>228</v>
       </c>
@@ -12389,7 +12389,7 @@
         <v>229</v>
       </c>
       <c r="R56" s="100"/>
-      <c r="T56" s="640"/>
+      <c r="T56" s="639"/>
       <c r="U56" s="364" t="s">
         <v>232</v>
       </c>
@@ -12399,7 +12399,7 @@
       <c r="W56" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="Y56" s="640"/>
+      <c r="Y56" s="639"/>
       <c r="Z56" s="364" t="s">
         <v>232</v>
       </c>
@@ -12623,18 +12623,18 @@
         <v>40</v>
       </c>
       <c r="R60" s="127"/>
-      <c r="T60" s="642" t="s">
+      <c r="T60" s="637" t="s">
         <v>274</v>
       </c>
-      <c r="U60" s="642"/>
-      <c r="V60" s="642"/>
-      <c r="W60" s="642"/>
-      <c r="Y60" s="642" t="s">
+      <c r="U60" s="637"/>
+      <c r="V60" s="637"/>
+      <c r="W60" s="637"/>
+      <c r="Y60" s="637" t="s">
         <v>275</v>
       </c>
-      <c r="Z60" s="642"/>
-      <c r="AA60" s="642"/>
-      <c r="AB60" s="642"/>
+      <c r="Z60" s="637"/>
+      <c r="AA60" s="637"/>
+      <c r="AB60" s="637"/>
     </row>
     <row r="61" spans="2:28" ht="19.5" customHeight="1">
       <c r="B61" s="150"/>
@@ -12818,7 +12818,7 @@
       <c r="R63" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="T63" s="639"/>
+      <c r="T63" s="640"/>
       <c r="U63" s="83" t="s">
         <v>212</v>
       </c>
@@ -12828,7 +12828,7 @@
       <c r="W63" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="Y63" s="639"/>
+      <c r="Y63" s="640"/>
       <c r="Z63" s="83" t="s">
         <v>212</v>
       </c>
@@ -12881,7 +12881,7 @@
       <c r="R64" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="T64" s="640"/>
+      <c r="T64" s="639"/>
       <c r="U64" s="83" t="s">
         <v>215</v>
       </c>
@@ -12891,7 +12891,7 @@
       <c r="W64" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="Y64" s="640"/>
+      <c r="Y64" s="639"/>
       <c r="Z64" s="83" t="s">
         <v>215</v>
       </c>
@@ -12970,7 +12970,7 @@
       </c>
     </row>
     <row r="66" spans="2:28">
-      <c r="T66" s="640"/>
+      <c r="T66" s="639"/>
       <c r="U66" s="81" t="s">
         <v>222</v>
       </c>
@@ -12980,7 +12980,7 @@
       <c r="W66" s="100" t="s">
         <v>266</v>
       </c>
-      <c r="Y66" s="640"/>
+      <c r="Y66" s="639"/>
       <c r="Z66" s="81" t="s">
         <v>222</v>
       </c>
@@ -13018,7 +13018,7 @@
       </c>
     </row>
     <row r="68" spans="2:28">
-      <c r="T68" s="639"/>
+      <c r="T68" s="640"/>
       <c r="U68" s="366" t="s">
         <v>228</v>
       </c>
@@ -13028,7 +13028,7 @@
       <c r="W68" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="Y68" s="639"/>
+      <c r="Y68" s="640"/>
       <c r="Z68" s="366" t="s">
         <v>228</v>
       </c>
@@ -13040,7 +13040,7 @@
       </c>
     </row>
     <row r="69" spans="2:28">
-      <c r="T69" s="640"/>
+      <c r="T69" s="639"/>
       <c r="U69" s="364" t="s">
         <v>232</v>
       </c>
@@ -13050,7 +13050,7 @@
       <c r="W69" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="Y69" s="640"/>
+      <c r="Y69" s="639"/>
       <c r="Z69" s="364" t="s">
         <v>232</v>
       </c>
@@ -13110,18 +13110,18 @@
       </c>
     </row>
     <row r="73" spans="2:28" ht="16.5" thickBot="1">
-      <c r="T73" s="637" t="s">
+      <c r="T73" s="642" t="s">
         <v>282</v>
       </c>
-      <c r="U73" s="637"/>
-      <c r="V73" s="637"/>
-      <c r="W73" s="637"/>
-      <c r="Y73" s="637" t="s">
+      <c r="U73" s="642"/>
+      <c r="V73" s="642"/>
+      <c r="W73" s="642"/>
+      <c r="Y73" s="642" t="s">
         <v>283</v>
       </c>
-      <c r="Z73" s="637"/>
-      <c r="AA73" s="637"/>
-      <c r="AB73" s="637"/>
+      <c r="Z73" s="642"/>
+      <c r="AA73" s="642"/>
+      <c r="AB73" s="642"/>
     </row>
     <row r="74" spans="2:28">
       <c r="T74" s="367" t="s">
@@ -13176,7 +13176,7 @@
       </c>
     </row>
     <row r="76" spans="2:28">
-      <c r="T76" s="639"/>
+      <c r="T76" s="640"/>
       <c r="U76" s="83" t="s">
         <v>212</v>
       </c>
@@ -13186,7 +13186,7 @@
       <c r="W76" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="Y76" s="639"/>
+      <c r="Y76" s="640"/>
       <c r="Z76" s="83" t="s">
         <v>212</v>
       </c>
@@ -13198,7 +13198,7 @@
       </c>
     </row>
     <row r="77" spans="2:28">
-      <c r="T77" s="640"/>
+      <c r="T77" s="639"/>
       <c r="U77" s="83" t="s">
         <v>215</v>
       </c>
@@ -13208,7 +13208,7 @@
       <c r="W77" s="100" t="s">
         <v>124</v>
       </c>
-      <c r="Y77" s="640"/>
+      <c r="Y77" s="639"/>
       <c r="Z77" s="83" t="s">
         <v>215</v>
       </c>
@@ -13246,7 +13246,7 @@
       </c>
     </row>
     <row r="79" spans="2:28">
-      <c r="T79" s="640"/>
+      <c r="T79" s="639"/>
       <c r="U79" s="81" t="s">
         <v>222</v>
       </c>
@@ -13256,7 +13256,7 @@
       <c r="W79" s="369" t="s">
         <v>286</v>
       </c>
-      <c r="Y79" s="640"/>
+      <c r="Y79" s="639"/>
       <c r="Z79" s="81" t="s">
         <v>222</v>
       </c>
@@ -13294,7 +13294,7 @@
       </c>
     </row>
     <row r="81" spans="20:28">
-      <c r="T81" s="639"/>
+      <c r="T81" s="640"/>
       <c r="U81" s="365" t="s">
         <v>228</v>
       </c>
@@ -13302,7 +13302,7 @@
         <v>229</v>
       </c>
       <c r="W81" s="370"/>
-      <c r="Y81" s="639"/>
+      <c r="Y81" s="640"/>
       <c r="Z81" s="365" t="s">
         <v>228</v>
       </c>
@@ -13312,7 +13312,7 @@
       <c r="AB81" s="370"/>
     </row>
     <row r="82" spans="20:28">
-      <c r="T82" s="640"/>
+      <c r="T82" s="639"/>
       <c r="U82" s="364" t="s">
         <v>232</v>
       </c>
@@ -13322,7 +13322,7 @@
       <c r="W82" s="369" t="s">
         <v>287</v>
       </c>
-      <c r="Y82" s="640"/>
+      <c r="Y82" s="639"/>
       <c r="Z82" s="364" t="s">
         <v>232</v>
       </c>
@@ -13383,6 +13383,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="Y73:AB73"/>
+    <mergeCell ref="Y75:Y77"/>
+    <mergeCell ref="Y78:Y79"/>
+    <mergeCell ref="Y80:Y82"/>
+    <mergeCell ref="Y83:Y84"/>
+    <mergeCell ref="Y60:AB60"/>
+    <mergeCell ref="Y62:Y64"/>
+    <mergeCell ref="Y65:Y66"/>
+    <mergeCell ref="Y67:Y69"/>
+    <mergeCell ref="Y70:Y71"/>
+    <mergeCell ref="Y47:AB47"/>
+    <mergeCell ref="Y49:Y51"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="Y54:Y56"/>
+    <mergeCell ref="Y57:Y58"/>
+    <mergeCell ref="Y34:AB34"/>
+    <mergeCell ref="Y36:Y38"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="Y41:Y43"/>
+    <mergeCell ref="Y44:Y45"/>
+    <mergeCell ref="T80:T82"/>
+    <mergeCell ref="T83:T84"/>
+    <mergeCell ref="T75:T77"/>
+    <mergeCell ref="T78:T79"/>
+    <mergeCell ref="T65:T66"/>
+    <mergeCell ref="T73:W73"/>
+    <mergeCell ref="T70:T71"/>
+    <mergeCell ref="T67:T69"/>
     <mergeCell ref="T34:W34"/>
     <mergeCell ref="T47:W47"/>
     <mergeCell ref="T60:W60"/>
@@ -13395,34 +13423,6 @@
     <mergeCell ref="T41:T43"/>
     <mergeCell ref="T44:T45"/>
     <mergeCell ref="T49:T51"/>
-    <mergeCell ref="T80:T82"/>
-    <mergeCell ref="T83:T84"/>
-    <mergeCell ref="T75:T77"/>
-    <mergeCell ref="T78:T79"/>
-    <mergeCell ref="T65:T66"/>
-    <mergeCell ref="T73:W73"/>
-    <mergeCell ref="T70:T71"/>
-    <mergeCell ref="T67:T69"/>
-    <mergeCell ref="Y34:AB34"/>
-    <mergeCell ref="Y36:Y38"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="Y41:Y43"/>
-    <mergeCell ref="Y44:Y45"/>
-    <mergeCell ref="Y47:AB47"/>
-    <mergeCell ref="Y49:Y51"/>
-    <mergeCell ref="Y52:Y53"/>
-    <mergeCell ref="Y54:Y56"/>
-    <mergeCell ref="Y57:Y58"/>
-    <mergeCell ref="Y60:AB60"/>
-    <mergeCell ref="Y62:Y64"/>
-    <mergeCell ref="Y65:Y66"/>
-    <mergeCell ref="Y67:Y69"/>
-    <mergeCell ref="Y70:Y71"/>
-    <mergeCell ref="Y73:AB73"/>
-    <mergeCell ref="Y75:Y77"/>
-    <mergeCell ref="Y78:Y79"/>
-    <mergeCell ref="Y80:Y82"/>
-    <mergeCell ref="Y83:Y84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="25" orientation="portrait" r:id="rId1"/>
@@ -15009,6 +15009,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B16:G16"/>
     <mergeCell ref="B51:K51"/>
     <mergeCell ref="B63:G63"/>
     <mergeCell ref="B64:G64"/>
@@ -15019,12 +15025,6 @@
     <mergeCell ref="B48:G48"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B35:I35"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
@@ -16605,11 +16605,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B51:K51"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="G56:K56"/>
     <mergeCell ref="B49:G49"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B15:G15"/>
@@ -16622,6 +16617,11 @@
     <mergeCell ref="B35:I35"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B51:K51"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="G56:K56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
@@ -16636,10 +16636,10 @@
   <dimension ref="B1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:W60"/>
+      <selection pane="bottomRight" activeCell="W60" sqref="A1:W60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
@@ -16672,7 +16672,7 @@
   <sheetData>
     <row r="1" spans="2:25" ht="30" thickBot="1">
       <c r="B1" s="514" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C1" s="514"/>
       <c r="E1" s="380"/>
@@ -16708,7 +16708,7 @@
         <v>62</v>
       </c>
       <c r="I2" s="418">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="J2" s="421" t="s">
         <v>318</v>
@@ -16720,13 +16720,13 @@
         <v>359</v>
       </c>
       <c r="M2" s="418">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N2" s="423" t="s">
         <v>66</v>
       </c>
       <c r="O2" s="419">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P2" s="424" t="s">
         <v>320</v>
@@ -16738,7 +16738,7 @@
         <v>321</v>
       </c>
       <c r="S2" s="425">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="X2" s="405"/>
       <c r="Y2" s="405"/>
@@ -16802,14 +16802,14 @@
       </c>
       <c r="O4" s="433">
         <f>N4*O2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="P4" s="434"/>
       <c r="Q4" s="435"/>
       <c r="R4" s="427"/>
       <c r="S4" s="464"/>
       <c r="U4" s="512" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="V4" s="508"/>
       <c r="W4" s="401"/>
@@ -16840,7 +16840,7 @@
       <c r="R5" s="427"/>
       <c r="S5" s="464"/>
       <c r="U5" s="512" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="V5" s="508"/>
       <c r="W5" s="401"/>
@@ -16913,7 +16913,7 @@
       </c>
       <c r="S7" s="436">
         <f>R7*S2</f>
-        <v>19.200000000000003</v>
+        <v>24</v>
       </c>
       <c r="T7" s="380"/>
       <c r="U7" s="508"/>
@@ -16950,7 +16950,7 @@
       </c>
       <c r="M8" s="519">
         <f>M2*L8</f>
-        <v>43.2</v>
+        <v>54</v>
       </c>
       <c r="N8" s="449"/>
       <c r="O8" s="450"/>
@@ -16997,7 +16997,7 @@
       </c>
       <c r="O9" s="433">
         <f>N9*O2</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P9" s="434"/>
       <c r="Q9" s="443"/>
@@ -17006,7 +17006,7 @@
       </c>
       <c r="S9" s="436">
         <f>R9*S2</f>
-        <v>2.4000000000000004</v>
+        <v>3</v>
       </c>
       <c r="T9" s="380"/>
       <c r="W9" s="401"/>
@@ -17041,7 +17041,7 @@
       </c>
       <c r="O10" s="519">
         <f>O2*N10</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P10" s="434"/>
       <c r="Q10" s="435"/>
@@ -17084,7 +17084,7 @@
       </c>
       <c r="M11" s="494">
         <f>M2*L11</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="N11" s="449"/>
       <c r="O11" s="450"/>
@@ -17095,7 +17095,7 @@
       </c>
       <c r="S11" s="436">
         <f>R11*S2</f>
-        <v>4.8000000000000007</v>
+        <v>6</v>
       </c>
       <c r="T11" s="380"/>
       <c r="U11" s="512" t="s">
@@ -17196,7 +17196,7 @@
       </c>
       <c r="O14" s="433">
         <f>N14*O2</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="P14" s="434"/>
       <c r="Q14" s="443"/>
@@ -17237,7 +17237,7 @@
       </c>
       <c r="O15" s="433">
         <f>N15*O2</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="P15" s="434"/>
       <c r="Q15" s="443"/>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="M17" s="518">
         <f>M2*L17</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="N17" s="604"/>
       <c r="O17" s="450"/>
@@ -17419,7 +17419,7 @@
       </c>
       <c r="O20" s="519">
         <f>O2*N20</f>
-        <v>19.200000000000003</v>
+        <v>24</v>
       </c>
       <c r="P20" s="434"/>
       <c r="Q20" s="435"/>
@@ -17457,7 +17457,7 @@
       <c r="S21" s="464"/>
       <c r="T21" s="380"/>
       <c r="U21" s="512" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="V21" s="508"/>
       <c r="W21" s="402"/>
@@ -17494,7 +17494,7 @@
       </c>
       <c r="O22" s="519">
         <f>O2*N22</f>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="P22" s="434"/>
       <c r="Q22" s="435"/>
@@ -17537,7 +17537,7 @@
       </c>
       <c r="O23" s="519">
         <f>O2*N23</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P23" s="434"/>
       <c r="Q23" s="435"/>
@@ -17578,7 +17578,7 @@
       </c>
       <c r="O24" s="553">
         <f>N24*O2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="P24" s="434"/>
       <c r="Q24" s="435"/>
@@ -17625,7 +17625,7 @@
       </c>
       <c r="S25" s="436">
         <f>R25*S2</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="T25" s="380"/>
       <c r="U25" s="512"/>
@@ -17662,7 +17662,7 @@
       </c>
       <c r="M26" s="494">
         <f>M2*L26</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="N26" s="449"/>
       <c r="O26" s="450"/>
@@ -17745,7 +17745,7 @@
       </c>
       <c r="S28" s="436">
         <f>R28*S2</f>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="T28" s="380"/>
       <c r="U28" s="512"/>
@@ -17784,7 +17784,7 @@
       </c>
       <c r="O29" s="433">
         <f>N29*O2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="P29" s="434"/>
       <c r="Q29" s="435"/>
@@ -17793,7 +17793,7 @@
       </c>
       <c r="S29" s="436">
         <f>R29*S2</f>
-        <v>4.8000000000000007</v>
+        <v>6</v>
       </c>
       <c r="T29" s="380"/>
       <c r="U29" s="512" t="s">
@@ -17834,7 +17834,7 @@
       </c>
       <c r="O30" s="519">
         <f>O2*N30</f>
-        <v>14.399999999999999</v>
+        <v>18</v>
       </c>
       <c r="P30" s="434"/>
       <c r="Q30" s="435"/>
@@ -17873,7 +17873,7 @@
       </c>
       <c r="M31" s="518">
         <f>L31*M2</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N31" s="552"/>
       <c r="O31" s="450"/>
@@ -18014,7 +18014,7 @@
       </c>
       <c r="O35" s="519">
         <f>N35*O2</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="P35" s="434"/>
       <c r="Q35" s="443"/>
@@ -18099,10 +18099,10 @@
       <c r="C38" s="427" t="s">
         <v>375</v>
       </c>
-      <c r="D38" s="601" t="s">
+      <c r="D38" s="532" t="s">
         <v>378</v>
       </c>
-      <c r="E38" s="602" t="s">
+      <c r="E38" s="467" t="s">
         <v>412</v>
       </c>
       <c r="F38" s="468"/>
@@ -18120,7 +18120,7 @@
       </c>
       <c r="O38" s="519">
         <f>N38*O2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="P38" s="434"/>
       <c r="Q38" s="443"/>
@@ -18142,10 +18142,10 @@
       <c r="C39" s="427" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="598" t="s">
+      <c r="D39" s="440" t="s">
         <v>150</v>
       </c>
-      <c r="E39" s="598" t="s">
+      <c r="E39" s="440" t="s">
         <v>356</v>
       </c>
       <c r="F39" s="438" t="s">
@@ -18168,7 +18168,8 @@
         <v>1.5</v>
       </c>
       <c r="S39" s="599">
-        <v>1.5</v>
+        <f>R39*S2</f>
+        <v>45</v>
       </c>
       <c r="T39" s="380"/>
       <c r="X39" s="405"/>
@@ -18235,7 +18236,7 @@
       </c>
       <c r="S41" s="436">
         <f>R41*S2</f>
-        <v>21.6</v>
+        <v>27</v>
       </c>
       <c r="T41" s="380"/>
       <c r="X41" s="405"/>
@@ -18294,7 +18295,7 @@
       </c>
       <c r="M43" s="518">
         <f>L43*M2</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N43" s="552"/>
       <c r="O43" s="450"/>
@@ -18361,7 +18362,7 @@
       </c>
       <c r="O45" s="519">
         <f>O2*N45</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="P45" s="434"/>
       <c r="Q45" s="435"/>
@@ -18397,7 +18398,7 @@
       </c>
       <c r="M46" s="519">
         <f>L46*M2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="N46" s="449"/>
       <c r="O46" s="450"/>
@@ -18439,7 +18440,7 @@
       </c>
       <c r="O47" s="433">
         <f>N47*O2</f>
-        <v>14.399999999999999</v>
+        <v>18</v>
       </c>
       <c r="P47" s="434"/>
       <c r="Q47" s="435"/>
@@ -18504,7 +18505,7 @@
       </c>
       <c r="M49" s="494">
         <f>L49*M2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="N49" s="435"/>
       <c r="O49" s="450"/>
@@ -18550,7 +18551,7 @@
       </c>
       <c r="S50" s="436">
         <f>R50*S2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="T50" s="380"/>
       <c r="X50" s="405"/>
@@ -18607,7 +18608,7 @@
       </c>
       <c r="I52" s="452">
         <f>H52*I2</f>
-        <v>28.799999999999997</v>
+        <v>36</v>
       </c>
       <c r="J52" s="427"/>
       <c r="K52" s="471"/>
@@ -18714,7 +18715,7 @@
       </c>
       <c r="O55" s="433">
         <f>N55*O2</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="P55" s="434"/>
       <c r="Q55" s="435"/>
@@ -18750,7 +18751,7 @@
       </c>
       <c r="M56" s="554">
         <f>L56*M2</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="N56" s="530"/>
       <c r="O56" s="503"/>
@@ -18788,7 +18789,7 @@
       </c>
       <c r="M57" s="556">
         <f>L57*M2</f>
-        <v>273.59999999999997</v>
+        <v>341.99999999999994</v>
       </c>
       <c r="N57" s="485">
         <f>SUM(N4:N56)</f>
@@ -18796,7 +18797,7 @@
       </c>
       <c r="O57" s="486">
         <f>N57*O2</f>
-        <v>400.7999999999999</v>
+        <v>500.99999999999989</v>
       </c>
       <c r="P57" s="487"/>
       <c r="Q57" s="488"/>
@@ -18806,7 +18807,7 @@
       </c>
       <c r="S57" s="490">
         <f>R57*S2</f>
-        <v>225.59999999999997</v>
+        <v>281.99999999999994</v>
       </c>
       <c r="Z57" s="381"/>
       <c r="AA57" s="403"/>
@@ -18837,7 +18838,7 @@
       </c>
       <c r="M58" s="555">
         <f>L58*M2</f>
-        <v>547.19999999999993</v>
+        <v>683.99999999999989</v>
       </c>
       <c r="N58" s="427">
         <f>N57*2</f>
@@ -18845,7 +18846,7 @@
       </c>
       <c r="O58" s="494">
         <f>N58*O2</f>
-        <v>801.5999999999998</v>
+        <v>1001.9999999999998</v>
       </c>
       <c r="P58" s="439"/>
       <c r="Q58" s="495"/>
@@ -18855,7 +18856,7 @@
       </c>
       <c r="S58" s="436">
         <f>R58*S2</f>
-        <v>451.19999999999993</v>
+        <v>563.99999999999989</v>
       </c>
       <c r="T58" s="380"/>
       <c r="X58" s="403"/>

</xml_diff>